<commit_message>
Updated Integration Tests Excel File
</commit_message>
<xml_diff>
--- a/src/integrationTest/resources/ServiceToIDAMRoleMapping_newRoles.xlsx
+++ b/src/integrationTest/resources/ServiceToIDAMRoleMapping_newRoles.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10912"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10215"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/m_2035593/tasks/hmcts/sourcecode/rd-caseworker-ref-api/src/integrationTest/resources/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/m_2109032/RDCC4025/rd-caseworker-ref-api/src/integrationTest/resources/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{70CB0E2D-F07A-2F4E-9401-F41FA782CC9E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BA417884-F0A3-5E4C-A084-6D3C9A40A92E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2460" yWindow="2480" windowWidth="17080" windowHeight="18740" xr2:uid="{B23E73D9-D44C-4ADD-8708-F0F51E97D08F}"/>
+    <workbookView xWindow="2460" yWindow="2480" windowWidth="17080" windowHeight="18740" activeTab="1" xr2:uid="{B23E73D9-D44C-4ADD-8708-F0F51E97D08F}"/>
   </bookViews>
   <sheets>
     <sheet name="Service to CW Roles Mapping" sheetId="1" r:id="rId1"/>
@@ -514,7 +514,7 @@
   </sheetPr>
   <dimension ref="A1:C14"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView topLeftCell="A20" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
@@ -692,7 +692,7 @@
   </sheetPr>
   <dimension ref="A1:B10"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>

</xml_diff>

<commit_message>
Updated functional Tests for RDCC-4134
</commit_message>
<xml_diff>
--- a/src/integrationTest/resources/ServiceToIDAMRoleMapping_newRoles.xlsx
+++ b/src/integrationTest/resources/ServiceToIDAMRoleMapping_newRoles.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10215"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10313"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/m_2109032/RDCC4025/rd-caseworker-ref-api/src/integrationTest/resources/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BA417884-F0A3-5E4C-A084-6D3C9A40A92E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5F5EEBAF-87C0-6348-9D75-20763628F168}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="2460" yWindow="2480" windowWidth="17080" windowHeight="18740" activeTab="1" xr2:uid="{B23E73D9-D44C-4ADD-8708-F0F51E97D08F}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="39" uniqueCount="19">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="44" uniqueCount="24">
   <si>
     <t>Service ID</t>
   </si>
@@ -66,38 +66,53 @@
     <t>caseworker-iac-dwp</t>
   </si>
   <si>
-    <t>Hearing Centre Team Leader </t>
-  </si>
-  <si>
     <t>Hearing Centre Administrator</t>
   </si>
   <si>
     <t>Court Clerk</t>
   </si>
   <si>
-    <t>National Business Centre Team leader</t>
-  </si>
-  <si>
-    <t>National Business Centre Listing team</t>
-  </si>
-  <si>
-    <t>National Business Centre Payments team</t>
-  </si>
-  <si>
-    <t>CTSC team leader</t>
-  </si>
-  <si>
     <t>CTSC Administrator</t>
   </si>
   <si>
     <t>BFA1</t>
+  </si>
+  <si>
+    <t>Hearing Centre Team Leader</t>
+  </si>
+  <si>
+    <t>National Business Centre Team Leader</t>
+  </si>
+  <si>
+    <t>National Business Centre Administrator</t>
+  </si>
+  <si>
+    <t>National Business Centre Listing Team</t>
+  </si>
+  <si>
+    <t>National Business Centre Payments Team</t>
+  </si>
+  <si>
+    <t>CTSC Team Leader</t>
+  </si>
+  <si>
+    <t>Regional Centre Team Leader</t>
+  </si>
+  <si>
+    <t>Regional Centre Administrator</t>
+  </si>
+  <si>
+    <t>DWP Administrator</t>
+  </si>
+  <si>
+    <t>HMRC Administrator</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="5" x14ac:knownFonts="1">
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -128,7 +143,14 @@
     </font>
     <font>
       <sz val="10"/>
-      <color theme="1"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -155,12 +177,12 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="7"/>
-        <bgColor indexed="64"/>
+        <fgColor rgb="FFFFC000"/>
+        <bgColor rgb="FF000000"/>
       </patternFill>
     </fill>
   </fills>
-  <borders count="2">
+  <borders count="3">
     <border>
       <left/>
       <right/>
@@ -183,6 +205,19 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
@@ -190,10 +225,12 @@
       <alignment horizontal="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="4" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -538,7 +575,7 @@
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>18</v>
+        <v>13</v>
       </c>
       <c r="B2">
         <v>1</v>
@@ -549,7 +586,7 @@
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>18</v>
+        <v>13</v>
       </c>
       <c r="B3">
         <v>1</v>
@@ -560,7 +597,7 @@
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
-        <v>18</v>
+        <v>13</v>
       </c>
       <c r="B4">
         <v>2</v>
@@ -571,7 +608,7 @@
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
-        <v>18</v>
+        <v>13</v>
       </c>
       <c r="B5">
         <v>2</v>
@@ -582,7 +619,7 @@
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
-        <v>18</v>
+        <v>13</v>
       </c>
       <c r="B6">
         <v>1</v>
@@ -593,7 +630,7 @@
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
-        <v>18</v>
+        <v>13</v>
       </c>
       <c r="B7">
         <v>3</v>
@@ -604,7 +641,7 @@
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
-        <v>18</v>
+        <v>13</v>
       </c>
       <c r="B8">
         <v>4</v>
@@ -615,7 +652,7 @@
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
-        <v>18</v>
+        <v>13</v>
       </c>
       <c r="B9">
         <v>5</v>
@@ -626,7 +663,7 @@
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
-        <v>18</v>
+        <v>13</v>
       </c>
       <c r="B10">
         <v>6</v>
@@ -637,7 +674,7 @@
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
-        <v>18</v>
+        <v>13</v>
       </c>
       <c r="B11">
         <v>7</v>
@@ -648,7 +685,7 @@
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
-        <v>18</v>
+        <v>13</v>
       </c>
       <c r="B12">
         <v>8</v>
@@ -659,7 +696,7 @@
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
-        <v>18</v>
+        <v>13</v>
       </c>
       <c r="B13">
         <v>9</v>
@@ -670,7 +707,7 @@
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
-        <v>18</v>
+        <v>13</v>
       </c>
       <c r="B14">
         <v>10</v>
@@ -690,9 +727,11 @@
   <sheetPr>
     <tabColor theme="7"/>
   </sheetPr>
-  <dimension ref="A1:B10"/>
+  <dimension ref="A1:B15"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B21" sqref="B21"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
@@ -703,80 +742,120 @@
       <c r="A1" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="B1">
+      <c r="B1" s="3">
         <v>1</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A2" s="2" t="s">
+      <c r="A2" s="4" t="s">
         <v>4</v>
       </c>
-      <c r="B2">
+      <c r="B2" s="3">
         <v>2</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A3" s="2" t="s">
+      <c r="A3" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="B3" s="3">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A4" s="4" t="s">
         <v>10</v>
       </c>
-      <c r="B3">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A4" s="2" t="s">
+      <c r="B4" s="3">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A5" s="4" t="s">
         <v>11</v>
       </c>
-      <c r="B4">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A5" s="2" t="s">
+      <c r="B5" s="3">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A6" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="B6" s="3">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A7" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="B7" s="3">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A8" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="B8" s="3">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A9" s="4" t="s">
+        <v>18</v>
+      </c>
+      <c r="B9" s="3">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A10" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="B10" s="3">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A11" s="4" t="s">
         <v>12</v>
       </c>
-      <c r="B5">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A6" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="B6">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A7" s="2" t="s">
+      <c r="B11" s="3">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="12" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A12" s="4" t="s">
+        <v>20</v>
+      </c>
+      <c r="B12" s="3">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="13" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A13" s="4" t="s">
+        <v>21</v>
+      </c>
+      <c r="B13" s="3">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="14" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A14" s="4" t="s">
+        <v>22</v>
+      </c>
+      <c r="B14" s="3">
         <v>14</v>
       </c>
-      <c r="B7">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A8" s="2" t="s">
+    </row>
+    <row r="15" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A15" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="B15" s="3">
         <v>15</v>
-      </c>
-      <c r="B8">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A9" s="2" t="s">
-        <v>16</v>
-      </c>
-      <c r="B9">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A10" s="2" t="s">
-        <v>17</v>
-      </c>
-      <c r="B10">
-        <v>10</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Rdcc 4134-SRD: Add new roles and user type for SSCS Hearings (#450)
 Updated for RDCC-4309
</commit_message>
<xml_diff>
--- a/src/integrationTest/resources/ServiceToIDAMRoleMapping_newRoles.xlsx
+++ b/src/integrationTest/resources/ServiceToIDAMRoleMapping_newRoles.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10215"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10313"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/m_2109032/RDCC4025/rd-caseworker-ref-api/src/integrationTest/resources/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BA417884-F0A3-5E4C-A084-6D3C9A40A92E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5F5EEBAF-87C0-6348-9D75-20763628F168}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="2460" yWindow="2480" windowWidth="17080" windowHeight="18740" activeTab="1" xr2:uid="{B23E73D9-D44C-4ADD-8708-F0F51E97D08F}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="39" uniqueCount="19">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="44" uniqueCount="24">
   <si>
     <t>Service ID</t>
   </si>
@@ -66,38 +66,53 @@
     <t>caseworker-iac-dwp</t>
   </si>
   <si>
-    <t>Hearing Centre Team Leader </t>
-  </si>
-  <si>
     <t>Hearing Centre Administrator</t>
   </si>
   <si>
     <t>Court Clerk</t>
   </si>
   <si>
-    <t>National Business Centre Team leader</t>
-  </si>
-  <si>
-    <t>National Business Centre Listing team</t>
-  </si>
-  <si>
-    <t>National Business Centre Payments team</t>
-  </si>
-  <si>
-    <t>CTSC team leader</t>
-  </si>
-  <si>
     <t>CTSC Administrator</t>
   </si>
   <si>
     <t>BFA1</t>
+  </si>
+  <si>
+    <t>Hearing Centre Team Leader</t>
+  </si>
+  <si>
+    <t>National Business Centre Team Leader</t>
+  </si>
+  <si>
+    <t>National Business Centre Administrator</t>
+  </si>
+  <si>
+    <t>National Business Centre Listing Team</t>
+  </si>
+  <si>
+    <t>National Business Centre Payments Team</t>
+  </si>
+  <si>
+    <t>CTSC Team Leader</t>
+  </si>
+  <si>
+    <t>Regional Centre Team Leader</t>
+  </si>
+  <si>
+    <t>Regional Centre Administrator</t>
+  </si>
+  <si>
+    <t>DWP Administrator</t>
+  </si>
+  <si>
+    <t>HMRC Administrator</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="5" x14ac:knownFonts="1">
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -128,7 +143,14 @@
     </font>
     <font>
       <sz val="10"/>
-      <color theme="1"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -155,12 +177,12 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="7"/>
-        <bgColor indexed="64"/>
+        <fgColor rgb="FFFFC000"/>
+        <bgColor rgb="FF000000"/>
       </patternFill>
     </fill>
   </fills>
-  <borders count="2">
+  <borders count="3">
     <border>
       <left/>
       <right/>
@@ -183,6 +205,19 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
@@ -190,10 +225,12 @@
       <alignment horizontal="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="4" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -538,7 +575,7 @@
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>18</v>
+        <v>13</v>
       </c>
       <c r="B2">
         <v>1</v>
@@ -549,7 +586,7 @@
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>18</v>
+        <v>13</v>
       </c>
       <c r="B3">
         <v>1</v>
@@ -560,7 +597,7 @@
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
-        <v>18</v>
+        <v>13</v>
       </c>
       <c r="B4">
         <v>2</v>
@@ -571,7 +608,7 @@
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
-        <v>18</v>
+        <v>13</v>
       </c>
       <c r="B5">
         <v>2</v>
@@ -582,7 +619,7 @@
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
-        <v>18</v>
+        <v>13</v>
       </c>
       <c r="B6">
         <v>1</v>
@@ -593,7 +630,7 @@
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
-        <v>18</v>
+        <v>13</v>
       </c>
       <c r="B7">
         <v>3</v>
@@ -604,7 +641,7 @@
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
-        <v>18</v>
+        <v>13</v>
       </c>
       <c r="B8">
         <v>4</v>
@@ -615,7 +652,7 @@
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
-        <v>18</v>
+        <v>13</v>
       </c>
       <c r="B9">
         <v>5</v>
@@ -626,7 +663,7 @@
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
-        <v>18</v>
+        <v>13</v>
       </c>
       <c r="B10">
         <v>6</v>
@@ -637,7 +674,7 @@
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
-        <v>18</v>
+        <v>13</v>
       </c>
       <c r="B11">
         <v>7</v>
@@ -648,7 +685,7 @@
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
-        <v>18</v>
+        <v>13</v>
       </c>
       <c r="B12">
         <v>8</v>
@@ -659,7 +696,7 @@
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
-        <v>18</v>
+        <v>13</v>
       </c>
       <c r="B13">
         <v>9</v>
@@ -670,7 +707,7 @@
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
-        <v>18</v>
+        <v>13</v>
       </c>
       <c r="B14">
         <v>10</v>
@@ -690,9 +727,11 @@
   <sheetPr>
     <tabColor theme="7"/>
   </sheetPr>
-  <dimension ref="A1:B10"/>
+  <dimension ref="A1:B15"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B21" sqref="B21"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
@@ -703,80 +742,120 @@
       <c r="A1" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="B1">
+      <c r="B1" s="3">
         <v>1</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A2" s="2" t="s">
+      <c r="A2" s="4" t="s">
         <v>4</v>
       </c>
-      <c r="B2">
+      <c r="B2" s="3">
         <v>2</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A3" s="2" t="s">
+      <c r="A3" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="B3" s="3">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A4" s="4" t="s">
         <v>10</v>
       </c>
-      <c r="B3">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A4" s="2" t="s">
+      <c r="B4" s="3">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A5" s="4" t="s">
         <v>11</v>
       </c>
-      <c r="B4">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A5" s="2" t="s">
+      <c r="B5" s="3">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A6" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="B6" s="3">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A7" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="B7" s="3">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A8" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="B8" s="3">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A9" s="4" t="s">
+        <v>18</v>
+      </c>
+      <c r="B9" s="3">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A10" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="B10" s="3">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A11" s="4" t="s">
         <v>12</v>
       </c>
-      <c r="B5">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A6" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="B6">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A7" s="2" t="s">
+      <c r="B11" s="3">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="12" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A12" s="4" t="s">
+        <v>20</v>
+      </c>
+      <c r="B12" s="3">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="13" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A13" s="4" t="s">
+        <v>21</v>
+      </c>
+      <c r="B13" s="3">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="14" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A14" s="4" t="s">
+        <v>22</v>
+      </c>
+      <c r="B14" s="3">
         <v>14</v>
       </c>
-      <c r="B7">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A8" s="2" t="s">
+    </row>
+    <row r="15" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A15" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="B15" s="3">
         <v>15</v>
-      </c>
-      <c r="B8">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A9" s="2" t="s">
-        <v>16</v>
-      </c>
-      <c r="B9">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A10" s="2" t="s">
-        <v>17</v>
-      </c>
-      <c r="B10">
-        <v>10</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
RDCC-4669: updated excel test files
</commit_message>
<xml_diff>
--- a/src/integrationTest/resources/ServiceToIDAMRoleMapping_newRoles.xlsx
+++ b/src/integrationTest/resources/ServiceToIDAMRoleMapping_newRoles.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10313"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11010"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/m_2109032/RDCC4025/rd-caseworker-ref-api/src/integrationTest/resources/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/m_900458/Documents/HMCTS/rd-caseworker-ref-api/src/integrationTest/resources/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5F5EEBAF-87C0-6348-9D75-20763628F168}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{91C07FE7-9729-5944-A913-D255445FE7CA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2460" yWindow="2480" windowWidth="17080" windowHeight="18740" activeTab="1" xr2:uid="{B23E73D9-D44C-4ADD-8708-F0F51E97D08F}"/>
+    <workbookView xWindow="2460" yWindow="460" windowWidth="17080" windowHeight="16440" activeTab="1" xr2:uid="{B23E73D9-D44C-4ADD-8708-F0F51E97D08F}"/>
   </bookViews>
   <sheets>
     <sheet name="Service to CW Roles Mapping" sheetId="1" r:id="rId1"/>
@@ -24,9 +24,7 @@
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
         <xcalcf:feature name="microsoft.com:RD"/>
-        <xcalcf:feature name="microsoft.com:Single"/>
         <xcalcf:feature name="microsoft.com:FV"/>
-        <xcalcf:feature name="microsoft.com:CNMTM"/>
       </xcalcf:calcFeatures>
     </ext>
   </extLst>
@@ -45,12 +43,6 @@
     <t>Role</t>
   </si>
   <si>
-    <t>Senior Tribunal Caseworker</t>
-  </si>
-  <si>
-    <t>Tribunal Caseworker</t>
-  </si>
-  <si>
     <t>caseworker-iac</t>
   </si>
   <si>
@@ -106,6 +98,12 @@
   </si>
   <si>
     <t>HMRC Administrator</t>
+  </si>
+  <si>
+    <t>Senior Legal Caseworker</t>
+  </si>
+  <si>
+    <t>Legal Caseworker</t>
   </si>
 </sst>
 </file>
@@ -575,145 +573,145 @@
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="B2">
         <v>1</v>
       </c>
       <c r="C2" t="s">
-        <v>5</v>
+        <v>3</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="B3">
         <v>1</v>
       </c>
       <c r="C3" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="B4">
         <v>2</v>
       </c>
       <c r="C4" t="s">
-        <v>6</v>
+        <v>4</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="B5">
         <v>2</v>
       </c>
       <c r="C5" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="B6">
         <v>1</v>
       </c>
       <c r="C6" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="B7">
         <v>3</v>
       </c>
       <c r="C7" t="s">
-        <v>5</v>
+        <v>3</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="B8">
         <v>4</v>
       </c>
       <c r="C8" t="s">
-        <v>5</v>
+        <v>3</v>
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="B9">
         <v>5</v>
       </c>
       <c r="C9" t="s">
-        <v>5</v>
+        <v>3</v>
       </c>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="B10">
         <v>6</v>
       </c>
       <c r="C10" t="s">
-        <v>5</v>
+        <v>3</v>
       </c>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="B11">
         <v>7</v>
       </c>
       <c r="C11" t="s">
-        <v>5</v>
+        <v>3</v>
       </c>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="B12">
         <v>8</v>
       </c>
       <c r="C12" t="s">
-        <v>5</v>
+        <v>3</v>
       </c>
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="B13">
         <v>9</v>
       </c>
       <c r="C13" t="s">
-        <v>5</v>
+        <v>3</v>
       </c>
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="B14">
         <v>10</v>
       </c>
       <c r="C14" t="s">
-        <v>5</v>
+        <v>3</v>
       </c>
     </row>
   </sheetData>
@@ -730,7 +728,7 @@
   <dimension ref="A1:B15"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B21" sqref="B21"/>
+      <selection activeCell="A5" sqref="A5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -740,7 +738,7 @@
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A1" s="2" t="s">
-        <v>3</v>
+        <v>22</v>
       </c>
       <c r="B1" s="3">
         <v>1</v>
@@ -748,7 +746,7 @@
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A2" s="4" t="s">
-        <v>4</v>
+        <v>23</v>
       </c>
       <c r="B2" s="3">
         <v>2</v>
@@ -756,7 +754,7 @@
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A3" s="4" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="B3" s="3">
         <v>3</v>
@@ -764,7 +762,7 @@
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A4" s="4" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="B4" s="3">
         <v>4</v>
@@ -772,7 +770,7 @@
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A5" s="4" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="B5" s="3">
         <v>5</v>
@@ -780,7 +778,7 @@
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A6" s="4" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="B6" s="3">
         <v>6</v>
@@ -788,7 +786,7 @@
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A7" s="4" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="B7" s="3">
         <v>11</v>
@@ -796,7 +794,7 @@
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A8" s="4" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="B8" s="3">
         <v>7</v>
@@ -804,7 +802,7 @@
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A9" s="4" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="B9" s="3">
         <v>8</v>
@@ -812,7 +810,7 @@
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A10" s="4" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="B10" s="3">
         <v>9</v>
@@ -820,7 +818,7 @@
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A11" s="4" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="B11" s="3">
         <v>10</v>
@@ -828,7 +826,7 @@
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A12" s="4" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="B12" s="3">
         <v>12</v>
@@ -836,7 +834,7 @@
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A13" s="4" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="B13" s="3">
         <v>13</v>
@@ -844,7 +842,7 @@
     </row>
     <row r="14" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A14" s="4" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="B14" s="3">
         <v>14</v>
@@ -852,7 +850,7 @@
     </row>
     <row r="15" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A15" s="4" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="B15" s="3">
         <v>15</v>

</xml_diff>